<commit_message>
updated template and now it also generates the names
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/repos/bracket-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CD9E2E-04E5-C745-8DDF-95EE90982BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752E5118-0491-154D-B871-7480B1817848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Tree" sheetId="5" r:id="rId3"/>
     <sheet name="Pool Matches" sheetId="6" r:id="rId4"/>
     <sheet name="Elimination Matches" sheetId="7" r:id="rId5"/>
+    <sheet name="Names to Print" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -112,6 +113,20 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -196,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,6 +224,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -221,6 +242,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -1592,13 +1616,13 @@
   <sheetData>
     <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
@@ -1711,23 +1735,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1735,4 +1759,24 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA952CF-7580-BA4A-BFF2-63054D7F5497}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="114" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="161.1640625" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added ability to create  knockout competitions
Also simplified large parts of the code and separated a bit more
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/repos/bracket-creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328B686-C409-6146-B04C-6C5C8B7D05B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032F262B-675A-DB45-8FD2-8AB8F864E70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -229,6 +229,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,12 +247,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1618,13 +1618,13 @@
   <sheetData>
     <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
@@ -1678,14 +1678,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4065E12-1BC4-BF48-9DCD-AFB9407081DC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1737,23 +1736,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1770,14 +1769,14 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="115" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="170.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="170.6640625" style="9" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData/>

</xml_diff>